<commit_message>
Tugas 4 database mysql
</commit_message>
<xml_diff>
--- a/TUGAS 4.xlsx
+++ b/TUGAS 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\Budi Luhur\Semester 6\PT Hendevane Indonesia\Database MySQL\tugas 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB035F83-2CEF-463F-BA95-B790BC4812B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2E2154-FF17-4C45-915F-11786070D7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{56760D18-AD64-4B41-B508-7FCCC2FC2036}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>id_pelatihan (PK)</t>
   </si>
@@ -33,9 +33,6 @@
     <t>nama_pelatihan</t>
   </si>
   <si>
-    <t>deskripsi_pelatihan</t>
-  </si>
-  <si>
     <t>tanggal_mulai</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
   </si>
   <si>
     <t>nomor_telepon</t>
-  </si>
-  <si>
-    <t>status_pembayaran</t>
   </si>
   <si>
     <t>id_presensi (PK)</t>
@@ -199,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -217,6 +211,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +534,7 @@
   <dimension ref="B3:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,12 +548,12 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -567,9 +567,6 @@
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -577,52 +574,47 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -652,24 +644,28 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>14</v>
+      <c r="F22" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -677,60 +673,63 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -738,7 +737,7 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
@@ -746,7 +745,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -754,7 +753,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
@@ -762,7 +761,7 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -770,11 +769,11 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -783,19 +782,19 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
@@ -835,11 +834,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B30:G30"/>
     <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>